<commit_message>
Added "required" message to sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Ranking choices.xlsx
+++ b/extras/sample-form/Ranking choices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/ranking-choices/extras/test-form/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/Finalized/ranking-choices/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DC3174-D1F8-0B42-950F-F306FD8DACCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C789B-1811-BB4E-B557-9ABCE115D267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27560" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="411">
   <si>
     <t>type</t>
   </si>
@@ -2681,9 +2681,6 @@
     <t>${all_disp}</t>
   </si>
   <si>
-    <t>jr:choice-name(selected-at(${ranked_crops}, ${rank} - 1), '${ranked_crops}')</t>
-  </si>
-  <si>
     <t>Bananas&lt;br&gt;Bananas!</t>
   </si>
   <si>
@@ -2715,6 +2712,12 @@
   </si>
   <si>
     <t>تمور</t>
+  </si>
+  <si>
+    <t>Please make at least one change to the ranking list before moving on, if even if you change it back.</t>
+  </si>
+  <si>
+    <t>choice-list(${ranked_crops}, selected-at(${ranked_crops}, ${rank} - 1))</t>
   </si>
 </sst>
 </file>
@@ -3163,7 +3166,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3279,6 +3282,7 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3312,7 +3316,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4865,11 +4872,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4911,7 +4918,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>363</v>
@@ -5124,44 +5131,32 @@
         <v>375</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="G11" s="65"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="65"/>
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>384</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>385</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>386</v>
       </c>
-      <c r="D11" t="s">
-        <v>401</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="D12" t="s">
         <v>400</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="L11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>402</v>
+      <c r="G12" t="s">
+        <v>399</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>360</v>
@@ -5169,22 +5164,34 @@
       <c r="K12" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="P12" t="s">
-        <v>382</v>
+      <c r="L12" t="s">
+        <v>387</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="O13" t="s">
-        <v>310</v>
+      <c r="K13" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="P13" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -5192,13 +5199,13 @@
         <v>139</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>360</v>
       </c>
       <c r="O14" t="s">
-        <v>398</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -5206,46 +5213,60 @@
         <v>139</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>360</v>
       </c>
       <c r="O15" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="O16" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>394</v>
-      </c>
-      <c r="O17" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" t="s">
+        <v>394</v>
+      </c>
+      <c r="O18" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>396</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>397</v>
       </c>
-      <c r="D18"/>
-      <c r="L18" t="s">
+      <c r="D19"/>
+      <c r="L19" t="s">
         <v>375</v>
       </c>
     </row>
@@ -5423,7 +5444,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>18</v>
@@ -5443,7 +5464,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5457,7 +5478,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5470,8 +5491,8 @@
       <c r="C4" t="s">
         <v>378</v>
       </c>
-      <c r="D4" s="64" t="s">
-        <v>406</v>
+      <c r="D4" s="53" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5482,10 +5503,10 @@
         <v>379</v>
       </c>
       <c r="C5" t="s">
-        <v>399</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>407</v>
+        <v>398</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5499,7 +5520,7 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -5513,7 +5534,7 @@
         <v>383</v>
       </c>
       <c r="D7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -5602,7 +5623,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2005121900</v>
+        <v>2105241708</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>360</v>
@@ -5637,22 +5658,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -5846,10 +5867,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="60" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -8639,10 +8660,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="61" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="61"/>
+      <c r="B83" s="62"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -9802,20 +9823,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="59"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9890,28 +9911,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>

<commit_message>
Added demo of "allowdef" to sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Ranking choices.xlsx
+++ b/extras/sample-form/Ranking choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/Finalized/ranking-choices/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C789B-1811-BB4E-B557-9ABCE115D267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50A0045-40FA-9D4A-9F04-15B90626E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28080" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="414">
   <si>
     <t>type</t>
   </si>
@@ -2718,6 +2718,15 @@
   </si>
   <si>
     <t>choice-list(${ranked_crops}, selected-at(${ranked_crops}, ${rank} - 1))</t>
+  </si>
+  <si>
+    <t>randomized custom-rankingchoices(allowdef=1, numbers=1)</t>
+  </si>
+  <si>
+    <t>allowdef_example</t>
+  </si>
+  <si>
+    <t>This field has an &lt;code&gt;allowdef&lt;/code&gt; value of 1, so the enumerator can move forward without making a change. This is a risky design, because the enumerator could go to the next field without actually checking the order of the choices.</t>
   </si>
 </sst>
 </file>
@@ -3431,7 +3440,277 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="169">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4872,11 +5151,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5270,142 +5549,304 @@
         <v>375</v>
       </c>
     </row>
+    <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>384</v>
+      </c>
+      <c r="B21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C21" t="s">
+        <v>413</v>
+      </c>
+      <c r="D21"/>
+      <c r="G21" t="s">
+        <v>411</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="L21" t="s">
+        <v>387</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>409</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:D1048576 J1:J1048576 G1:G1048576">
-    <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 J1:J20 G1:G20 G22:G1048576 J22:J1048576 B22:D1048576">
+    <cfRule type="expression" dxfId="168" priority="84" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 P1:P1048576 J1:J1048576">
-    <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 P1:P20 J1:J20 J22:J1048576 P22:P1048576 B22:D1048576">
+    <cfRule type="expression" dxfId="167" priority="81" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E1048576 G1:G1048576">
-    <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E20 G1:G20 G22:G1048576 B22:E1048576">
+    <cfRule type="expression" dxfId="166" priority="78" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E1048576 H1:I1048576">
-    <cfRule type="expression" dxfId="130" priority="41" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E20 H1:I20 H22:I1048576 B22:E1048576">
+    <cfRule type="expression" dxfId="165" priority="76" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E1048576 H1:I1048576">
-    <cfRule type="expression" dxfId="129" priority="39" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E20 H1:I20 H22:I1048576 B22:E1048576">
+    <cfRule type="expression" dxfId="164" priority="74" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
-    <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 G1:G20 G22:G1048576 B22:D1048576">
+    <cfRule type="expression" dxfId="163" priority="69" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:G20 B1:B20 B22:B1048576 G22:G1048576">
+    <cfRule type="expression" dxfId="162" priority="59" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576">
-    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 B22:D1048576">
+    <cfRule type="expression" dxfId="161" priority="53" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="55" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="57" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="123" priority="16" stopIfTrue="1">
+  <conditionalFormatting sqref="O1:O20 B1:B20 B22:B1048576 O22:O1048576">
+    <cfRule type="expression" dxfId="158" priority="51" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
-    <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 G1:G20 G22:G1048576 B22:D1048576">
+    <cfRule type="expression" dxfId="157" priority="49" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
-    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 G1:G20 G22:G1048576 B22:D1048576">
+    <cfRule type="expression" dxfId="156" priority="45" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576">
-    <cfRule type="expression" dxfId="120" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D20 B22:D1048576">
+    <cfRule type="expression" dxfId="155" priority="43" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:X1048576">
-    <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:X20 A22:X1048576">
+    <cfRule type="expression" dxfId="154" priority="37" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="40" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="44" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="46" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="50" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="54" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="56" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="58" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="60" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="63" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="70" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="75" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="77" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="79" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="80" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="82" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="83" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="85" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B20 B22:B1048576">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 G1:G1048576">
-    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B20 G1:G20 G22:G1048576 B22:B1048576">
+    <cfRule type="expression" dxfId="134" priority="36" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21 J21 G21">
+    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
+      <formula>$A21="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21 P21 J21">
+    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
+      <formula>$A21="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:E21 G21">
+    <cfRule type="expression" dxfId="32" priority="28" stopIfTrue="1">
+      <formula>$A21="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:E21 H21:I21">
+    <cfRule type="expression" dxfId="31" priority="26" stopIfTrue="1">
+      <formula>$A21="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:E21 H21:I21">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+      <formula>$A21="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21 G21">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A21, 16)="select_multiple ", LEN($A21)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A21, 17)))), AND(LEFT($A21, 11)="select_one ", LEN($A21)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A21, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21 B21">
+    <cfRule type="expression" dxfId="28" priority="19" stopIfTrue="1">
+      <formula>OR($A21="audio audit", $A21="text audit", $A21="speed violations count", $A21="speed violations list", $A21="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21">
+    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+      <formula>$A21="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="15" stopIfTrue="1">
+      <formula>$A21="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+      <formula>OR($A21="geopoint", $A21="geoshape", $A21="geotrace")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O21 B21">
+    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
+      <formula>OR($A21="calculate", $A21="calculate_here")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21 G21">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
+      <formula>OR($A21="date", $A21="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21 G21">
+    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+      <formula>$A21="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D21">
+    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+      <formula>OR($A21="audio", $A21="video")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:X21">
+    <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A21, 14)="sensor_stream ", LEN($A21)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A21, 15)))), AND(LEFT($A21, 17)="sensor_statistic ", LEN($A21)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A21, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+      <formula>$A21="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+      <formula>OR($A21="audio", $A21="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
+      <formula>$A21="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
+      <formula>OR($A21="date", $A21="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
+      <formula>OR($A21="calculate", $A21="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
+      <formula>$A21="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+      <formula>$A21="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
+      <formula>OR($A21="geopoint", $A21="geoshape", $A21="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+      <formula>OR($A21="audio audit", $A21="text audit", $A21="speed violations count", $A21="speed violations list", $A21="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="21" stopIfTrue="1">
+      <formula>OR($A21="username", $A21="phonenumber", $A21="start", $A21="end", $A21="deviceid", $A21="subscriberid", $A21="simserial", $A21="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A21, 16)="select_multiple ", LEN($A21)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A21, 17)))), AND(LEFT($A21, 11)="select_one ", LEN($A21)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A21, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="25" stopIfTrue="1">
+      <formula>$A21="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
+      <formula>$A21="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="29" stopIfTrue="1">
+      <formula>$A21="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="30" stopIfTrue="1">
+      <formula>$A21="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="32" stopIfTrue="1">
+      <formula>$A21="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="33" stopIfTrue="1">
+      <formula>$A21="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="35" stopIfTrue="1">
+      <formula>$A21="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>$A21="comments"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 G21">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A21, 14)="sensor_stream ", LEN($A21)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A21, 15)))), AND(LEFT($A21, 17)="sensor_statistic ", LEN($A21)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A21, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5565,7 +6006,7 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:I2000">
-    <cfRule type="expression" dxfId="98" priority="1">
+    <cfRule type="expression" dxfId="133" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5623,7 +6064,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2105241708</v>
+        <v>2105251154</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>360</v>
@@ -9459,348 +9900,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>